<commit_message>
update Venn and CDR file
</commit_message>
<xml_diff>
--- a/data/Genome-wide screen refs.xlsx
+++ b/data/Genome-wide screen refs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbaeten/Desktop/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihan/Documents/GitHub/ts_machine_learning/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15810EA4-C86B-7941-BB9D-D7DDDD3400DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03B8D3E-FD07-4C4D-8667-5D67714CA529}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="27040" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2320" yWindow="2480" windowWidth="27040" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2754,10 +2756,10 @@
   <dimension ref="A1:IV30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3369,7 +3371,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="49">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D4" s="50" t="s">
         <v>11</v>

</xml_diff>